<commit_message>
add settings inf for connect to server
</commit_message>
<xml_diff>
--- a/BookShop2023/Assets/Data/Products.xlsx
+++ b/BookShop2023/Assets/Data/Products.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27930" windowHeight="12930" activeTab="1"/>
+    <workbookView windowWidth="12165" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="2" r:id="rId1"/>
     <sheet name="Products" sheetId="3" r:id="rId2"/>
+    <sheet name="OrderStatusEnum" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="251">
   <si>
     <t>Order</t>
   </si>
@@ -56,7 +57,10 @@
     <t>PublishedYear</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>PurchasePrice</t>
+  </si>
+  <si>
+    <t>SellingPrice</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -65,6 +69,9 @@
     <t>ImageName</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Tâm Lý Học Đời Sống</t>
   </si>
   <si>
@@ -717,6 +724,51 @@
   </si>
   <si>
     <t>76.jpg</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>DisplayText</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Đơn hàng mới được tạo</t>
+  </si>
+  <si>
+    <t>Mới tạo</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Khách hàng đã thanh toán</t>
+  </si>
+  <si>
+    <t>Đã thanh toán</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Đơn hàng đã hủy</t>
+  </si>
+  <si>
+    <t>Đã hủy</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Đã thanh toán và đã giao</t>
+  </si>
+  <si>
+    <t>Đã giao</t>
   </si>
 </sst>
 </file>
@@ -730,14 +782,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="#,##0;\-#,##0"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1193,148 +1238,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1668,8 +1713,8 @@
   <sheetPr/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1758,23 +1803,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="41.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="15.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="12.5714285714286" customWidth="1"/>
     <col min="6" max="6" width="11.8571428571429" style="1"/>
-    <col min="8" max="8" width="12.5714285714286" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.5714285714286" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1796,11 +1841,17 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1808,10 +1859,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>2020</v>
@@ -1819,14 +1870,18 @@
       <c r="F2" s="1">
         <v>99000</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
+        <f>F2+25000</f>
+        <v>124000</v>
+      </c>
+      <c r="H2">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1834,10 +1889,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>2019</v>
@@ -1845,14 +1900,18 @@
       <c r="F3" s="1">
         <v>179000</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G34" si="0">F3+25000</f>
+        <v>204000</v>
+      </c>
+      <c r="H3">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1860,10 +1919,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>2018</v>
@@ -1871,14 +1930,18 @@
       <c r="F4" s="1">
         <v>89000</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>114000</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1886,10 +1949,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>2017</v>
@@ -1897,14 +1960,18 @@
       <c r="F5" s="1">
         <v>79000</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>104000</v>
+      </c>
+      <c r="H5">
         <v>7</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1912,10 +1979,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6">
         <v>2016</v>
@@ -1923,14 +1990,18 @@
       <c r="F6" s="1">
         <v>85000</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="H6">
         <v>9</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1938,10 +2009,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>2018</v>
@@ -1949,14 +2020,18 @@
       <c r="F7" s="1">
         <v>69000</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H7">
         <v>13</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1964,10 +2039,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
       </c>
       <c r="E8">
         <v>2021</v>
@@ -1975,14 +2050,18 @@
       <c r="F8" s="1">
         <v>69000</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H8">
         <v>21</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1990,10 +2069,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E9">
         <v>2020</v>
@@ -2001,14 +2080,18 @@
       <c r="F9" s="1">
         <v>139000</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>164000</v>
+      </c>
+      <c r="H9">
         <v>17</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2016,10 +2099,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10">
         <v>2019</v>
@@ -2027,14 +2110,18 @@
       <c r="F10" s="1">
         <v>159000</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>184000</v>
+      </c>
+      <c r="H10">
         <v>19</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2042,10 +2129,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>2020</v>
@@ -2053,14 +2140,18 @@
       <c r="F11" s="1">
         <v>99000</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>124000</v>
+      </c>
+      <c r="H11">
         <v>53</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2068,10 +2159,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>2018</v>
@@ -2079,14 +2170,18 @@
       <c r="F12" s="1">
         <v>89000</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>114000</v>
+      </c>
+      <c r="H12">
         <v>16</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2094,10 +2189,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>2015</v>
@@ -2105,14 +2200,18 @@
       <c r="F13" s="1">
         <v>69000</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H13">
         <v>28</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2120,10 +2219,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>2020</v>
@@ -2131,14 +2230,18 @@
       <c r="F14" s="1">
         <v>99000</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>124000</v>
+      </c>
+      <c r="H14">
         <v>100</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2146,10 +2249,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
         <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
       </c>
       <c r="E15">
         <v>2019</v>
@@ -2157,14 +2260,18 @@
       <c r="F15" s="1">
         <v>179000</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>204000</v>
+      </c>
+      <c r="H15">
         <v>69</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2172,10 +2279,10 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E16">
         <v>2018</v>
@@ -2183,14 +2290,18 @@
       <c r="F16" s="1">
         <v>89000</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>114000</v>
+      </c>
+      <c r="H16">
         <v>73</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2198,10 +2309,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E17">
         <v>2017</v>
@@ -2209,14 +2320,18 @@
       <c r="F17" s="1">
         <v>79000</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>104000</v>
+      </c>
+      <c r="H17">
         <v>22</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2224,10 +2339,10 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
         <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
       </c>
       <c r="E18">
         <v>2016</v>
@@ -2235,14 +2350,18 @@
       <c r="F18" s="1">
         <v>85000</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="H18">
         <v>91</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2250,10 +2369,10 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E19">
         <v>2018</v>
@@ -2261,14 +2380,18 @@
       <c r="F19" s="1">
         <v>69000</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H19">
         <v>16</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2276,10 +2399,10 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E20">
         <v>2021</v>
@@ -2287,14 +2410,18 @@
       <c r="F20" s="1">
         <v>69000</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H20">
         <v>27</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2302,10 +2429,10 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E21">
         <v>2020</v>
@@ -2313,14 +2440,18 @@
       <c r="F21" s="1">
         <v>139000</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>164000</v>
+      </c>
+      <c r="H21">
         <v>85</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2328,10 +2459,10 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E22">
         <v>2019</v>
@@ -2339,14 +2470,18 @@
       <c r="F22" s="1">
         <v>159000</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>184000</v>
+      </c>
+      <c r="H22">
         <v>35</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2354,10 +2489,10 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E23">
         <v>2020</v>
@@ -2365,14 +2500,18 @@
       <c r="F23" s="1">
         <v>99000</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>124000</v>
+      </c>
+      <c r="H23">
         <v>96</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2380,10 +2519,10 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E24">
         <v>2018</v>
@@ -2391,14 +2530,18 @@
       <c r="F24" s="1">
         <v>89000</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>114000</v>
+      </c>
+      <c r="H24">
         <v>45</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2406,10 +2549,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E25">
         <v>2015</v>
@@ -2417,14 +2560,18 @@
       <c r="F25" s="1">
         <v>69000</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H25">
         <v>37</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2432,10 +2579,10 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E26">
         <v>2020</v>
@@ -2443,14 +2590,18 @@
       <c r="F26" s="1">
         <v>99000</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>124000</v>
+      </c>
+      <c r="H26">
         <v>100</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2458,10 +2609,10 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E27">
         <v>2019</v>
@@ -2469,14 +2620,18 @@
       <c r="F27" s="1">
         <v>179000</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>204000</v>
+      </c>
+      <c r="H27">
         <v>69</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2484,10 +2639,10 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E28">
         <v>2018</v>
@@ -2495,14 +2650,18 @@
       <c r="F28" s="1">
         <v>89000</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>114000</v>
+      </c>
+      <c r="H28">
         <v>73</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2510,10 +2669,10 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E29">
         <v>2017</v>
@@ -2521,14 +2680,18 @@
       <c r="F29" s="1">
         <v>79000</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>104000</v>
+      </c>
+      <c r="H29">
         <v>22</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2536,10 +2699,10 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E30">
         <v>2016</v>
@@ -2547,14 +2710,18 @@
       <c r="F30" s="1">
         <v>85000</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="H30">
         <v>91</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2562,10 +2729,10 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E31">
         <v>2018</v>
@@ -2573,14 +2740,18 @@
       <c r="F31" s="1">
         <v>69000</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H31">
         <v>16</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2588,10 +2759,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E32">
         <v>2021</v>
@@ -2599,14 +2770,18 @@
       <c r="F32" s="1">
         <v>69000</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
+        <f t="shared" si="0"/>
+        <v>94000</v>
+      </c>
+      <c r="H32">
         <v>27</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2614,10 +2789,10 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E33">
         <v>2020</v>
@@ -2625,14 +2800,18 @@
       <c r="F33" s="1">
         <v>139000</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
+        <f t="shared" si="0"/>
+        <v>164000</v>
+      </c>
+      <c r="H33">
         <v>85</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2640,10 +2819,10 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E34">
         <v>2019</v>
@@ -2651,14 +2830,18 @@
       <c r="F34" s="1">
         <v>159000</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
+        <v>184000</v>
+      </c>
+      <c r="H34">
         <v>35</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2666,10 +2849,10 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E35">
         <v>2020</v>
@@ -2677,14 +2860,18 @@
       <c r="F35" s="1">
         <v>99000</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
+        <f t="shared" ref="G35:G66" si="1">F35+25000</f>
+        <v>124000</v>
+      </c>
+      <c r="H35">
         <v>96</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2692,10 +2879,10 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E36">
         <v>2018</v>
@@ -2703,14 +2890,18 @@
       <c r="F36" s="1">
         <v>89000</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
+        <f t="shared" si="1"/>
+        <v>114000</v>
+      </c>
+      <c r="H36">
         <v>45</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2718,10 +2909,10 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E37">
         <v>2015</v>
@@ -2729,14 +2920,18 @@
       <c r="F37" s="1">
         <v>69000</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H37">
         <v>37</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2744,10 +2939,10 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E38">
         <v>2020</v>
@@ -2755,14 +2950,18 @@
       <c r="F38" s="1">
         <v>99000</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
+        <f t="shared" si="1"/>
+        <v>124000</v>
+      </c>
+      <c r="H38">
         <v>100</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2770,10 +2969,10 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E39">
         <v>2019</v>
@@ -2781,14 +2980,18 @@
       <c r="F39" s="1">
         <v>179000</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
+        <f t="shared" si="1"/>
+        <v>204000</v>
+      </c>
+      <c r="H39">
         <v>69</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2796,10 +2999,10 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E40">
         <v>2018</v>
@@ -2807,14 +3010,18 @@
       <c r="F40" s="1">
         <v>89000</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
+        <f t="shared" si="1"/>
+        <v>114000</v>
+      </c>
+      <c r="H40">
         <v>73</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2822,10 +3029,10 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E41">
         <v>2022</v>
@@ -2833,14 +3040,18 @@
       <c r="F41" s="1">
         <v>79000</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
+        <f t="shared" si="1"/>
+        <v>104000</v>
+      </c>
+      <c r="H41">
         <v>22</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2848,10 +3059,10 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E42">
         <v>2016</v>
@@ -2859,14 +3070,18 @@
       <c r="F42" s="1">
         <v>85000</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
+        <f t="shared" si="1"/>
+        <v>110000</v>
+      </c>
+      <c r="H42">
         <v>91</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2874,10 +3089,10 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E43">
         <v>2021</v>
@@ -2885,14 +3100,18 @@
       <c r="F43" s="1">
         <v>69000</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H43">
         <v>8</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2900,10 +3119,10 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E44">
         <v>2021</v>
@@ -2911,14 +3130,18 @@
       <c r="F44" s="1">
         <v>69000</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H44">
         <v>11</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2926,10 +3149,10 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E45">
         <v>2021</v>
@@ -2937,14 +3160,18 @@
       <c r="F45" s="1">
         <v>139000</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="1">
+        <f t="shared" si="1"/>
+        <v>164000</v>
+      </c>
+      <c r="H45">
         <v>8</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2952,10 +3179,10 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E46">
         <v>2022</v>
@@ -2963,14 +3190,18 @@
       <c r="F46" s="1">
         <v>159000</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="1">
+        <f t="shared" si="1"/>
+        <v>184000</v>
+      </c>
+      <c r="H46">
         <v>7</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2978,10 +3209,10 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E47">
         <v>2023</v>
@@ -2989,14 +3220,18 @@
       <c r="F47" s="1">
         <v>99000</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="1">
+        <f t="shared" si="1"/>
+        <v>124000</v>
+      </c>
+      <c r="H47">
         <v>4</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3004,10 +3239,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E48">
         <v>2021</v>
@@ -3015,14 +3250,18 @@
       <c r="F48" s="1">
         <v>89000</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="1">
+        <f t="shared" si="1"/>
+        <v>114000</v>
+      </c>
+      <c r="H48">
         <v>45</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3030,10 +3269,10 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D49" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E49">
         <v>2021</v>
@@ -3041,14 +3280,18 @@
       <c r="F49" s="1">
         <v>69000</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H49">
         <v>2</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3056,10 +3299,10 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E50">
         <v>2022</v>
@@ -3067,14 +3310,18 @@
       <c r="F50" s="1">
         <v>99000</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="1">
+        <f t="shared" si="1"/>
+        <v>124000</v>
+      </c>
+      <c r="H50">
         <v>4</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3082,10 +3329,10 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D51" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E51">
         <v>2023</v>
@@ -3093,14 +3340,18 @@
       <c r="F51" s="1">
         <v>179000</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="1">
+        <f t="shared" si="1"/>
+        <v>204000</v>
+      </c>
+      <c r="H51">
         <v>3</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3108,10 +3359,10 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D52" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E52">
         <v>2018</v>
@@ -3119,14 +3370,18 @@
       <c r="F52" s="1">
         <v>89000</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="1">
+        <f t="shared" si="1"/>
+        <v>114000</v>
+      </c>
+      <c r="H52">
         <v>73</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3134,10 +3389,10 @@
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D53" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E53">
         <v>2017</v>
@@ -3145,14 +3400,18 @@
       <c r="F53" s="1">
         <v>79000</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="1">
+        <f t="shared" si="1"/>
+        <v>104000</v>
+      </c>
+      <c r="H53">
         <v>22</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3160,10 +3419,10 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D54" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E54">
         <v>2016</v>
@@ -3171,14 +3430,18 @@
       <c r="F54" s="1">
         <v>85000</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="1">
+        <f t="shared" si="1"/>
+        <v>110000</v>
+      </c>
+      <c r="H54">
         <v>91</v>
       </c>
-      <c r="H54" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="I54" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3186,10 +3449,10 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D55" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E55">
         <v>2018</v>
@@ -3197,14 +3460,18 @@
       <c r="F55" s="1">
         <v>69000</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H55">
         <v>16</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="I55" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3212,10 +3479,10 @@
         <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D56" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E56">
         <v>2021</v>
@@ -3223,14 +3490,18 @@
       <c r="F56" s="1">
         <v>69000</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H56">
         <v>27</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3238,10 +3509,10 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E57">
         <v>2020</v>
@@ -3249,14 +3520,18 @@
       <c r="F57" s="1">
         <v>139000</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="1">
+        <f t="shared" si="1"/>
+        <v>164000</v>
+      </c>
+      <c r="H57">
         <v>85</v>
       </c>
-      <c r="H57" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="I57" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3264,10 +3539,10 @@
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D58" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E58">
         <v>2019</v>
@@ -3275,14 +3550,18 @@
       <c r="F58" s="1">
         <v>159000</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="1">
+        <f t="shared" si="1"/>
+        <v>184000</v>
+      </c>
+      <c r="H58">
         <v>35</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3290,10 +3569,10 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E59">
         <v>2020</v>
@@ -3301,14 +3580,18 @@
       <c r="F59" s="1">
         <v>99000</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="1">
+        <f t="shared" si="1"/>
+        <v>124000</v>
+      </c>
+      <c r="H59">
         <v>96</v>
       </c>
-      <c r="H59" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3316,10 +3599,10 @@
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E60">
         <v>2018</v>
@@ -3327,14 +3610,18 @@
       <c r="F60" s="1">
         <v>89000</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="1">
+        <f t="shared" si="1"/>
+        <v>114000</v>
+      </c>
+      <c r="H60">
         <v>45</v>
       </c>
-      <c r="H60" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3342,10 +3629,10 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D61" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E61">
         <v>2015</v>
@@ -3353,14 +3640,18 @@
       <c r="F61" s="1">
         <v>69000</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="1">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="H61">
         <v>37</v>
       </c>
-      <c r="H61" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="I61" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3368,10 +3659,10 @@
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D62" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E62">
         <v>2020</v>
@@ -3379,14 +3670,18 @@
       <c r="F62" s="1">
         <v>99000</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="1">
+        <f t="shared" si="1"/>
+        <v>124000</v>
+      </c>
+      <c r="H62">
         <v>100</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3394,10 +3689,10 @@
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D63" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E63">
         <v>2019</v>
@@ -3405,14 +3700,18 @@
       <c r="F63" s="1">
         <v>179000</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="1">
+        <f t="shared" si="1"/>
+        <v>204000</v>
+      </c>
+      <c r="H63">
         <v>69</v>
       </c>
-      <c r="H63" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="I63" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3420,10 +3719,10 @@
         <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D64" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E64">
         <v>2018</v>
@@ -3431,14 +3730,18 @@
       <c r="F64" s="1">
         <v>89000</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="1">
+        <f t="shared" si="1"/>
+        <v>114000</v>
+      </c>
+      <c r="H64">
         <v>73</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="I64" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3446,10 +3749,10 @@
         <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D65" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E65">
         <v>2017</v>
@@ -3457,14 +3760,18 @@
       <c r="F65" s="1">
         <v>79000</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="1">
+        <f t="shared" si="1"/>
+        <v>104000</v>
+      </c>
+      <c r="H65">
         <v>22</v>
       </c>
-      <c r="H65" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3472,10 +3779,10 @@
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D66" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E66">
         <v>2016</v>
@@ -3483,14 +3790,18 @@
       <c r="F66" s="1">
         <v>85000</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="1">
+        <f t="shared" si="1"/>
+        <v>110000</v>
+      </c>
+      <c r="H66">
         <v>91</v>
       </c>
-      <c r="H66" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="I66" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3498,10 +3809,10 @@
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D67" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E67">
         <v>2018</v>
@@ -3509,14 +3820,18 @@
       <c r="F67" s="1">
         <v>69000</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="1">
+        <f>F67+25000</f>
+        <v>94000</v>
+      </c>
+      <c r="H67">
         <v>16</v>
       </c>
-      <c r="H67" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="I67" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3524,10 +3839,10 @@
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D68" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E68">
         <v>2021</v>
@@ -3535,14 +3850,18 @@
       <c r="F68" s="1">
         <v>69000</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="1">
+        <f>F68+25000</f>
+        <v>94000</v>
+      </c>
+      <c r="H68">
         <v>27</v>
       </c>
-      <c r="H68" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3550,10 +3869,10 @@
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D69" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E69">
         <v>2020</v>
@@ -3561,14 +3880,18 @@
       <c r="F69" s="1">
         <v>139000</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="1">
+        <f>F69+25000</f>
+        <v>164000</v>
+      </c>
+      <c r="H69">
         <v>85</v>
       </c>
-      <c r="H69" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="I69" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3576,10 +3899,10 @@
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D70" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E70">
         <v>2019</v>
@@ -3587,14 +3910,18 @@
       <c r="F70" s="1">
         <v>159000</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="1">
+        <f>F70+25000</f>
+        <v>184000</v>
+      </c>
+      <c r="H70">
         <v>35</v>
       </c>
-      <c r="H70" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I70" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3602,10 +3929,10 @@
         <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E71">
         <v>2020</v>
@@ -3613,14 +3940,18 @@
       <c r="F71" s="1">
         <v>99000</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="1">
+        <f>F71+25000</f>
+        <v>124000</v>
+      </c>
+      <c r="H71">
         <v>96</v>
       </c>
-      <c r="H71" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3628,10 +3959,10 @@
         <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D72" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E72">
         <v>2018</v>
@@ -3639,14 +3970,18 @@
       <c r="F72" s="1">
         <v>89000</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="1">
+        <f>F72+25000</f>
+        <v>114000</v>
+      </c>
+      <c r="H72">
         <v>45</v>
       </c>
-      <c r="H72" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I72" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3654,10 +3989,10 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
+        <v>222</v>
+      </c>
+      <c r="D73" t="s">
         <v>220</v>
-      </c>
-      <c r="D73" t="s">
-        <v>218</v>
       </c>
       <c r="E73">
         <v>2015</v>
@@ -3665,14 +4000,18 @@
       <c r="F73" s="1">
         <v>69000</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="1">
+        <f>F73+25000</f>
+        <v>94000</v>
+      </c>
+      <c r="H73">
         <v>37</v>
       </c>
-      <c r="H73" s="3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="I73" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3680,10 +4019,10 @@
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E74">
         <v>2020</v>
@@ -3691,14 +4030,18 @@
       <c r="F74" s="1">
         <v>99000</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="1">
+        <f>F74+25000</f>
+        <v>124000</v>
+      </c>
+      <c r="H74">
         <v>100</v>
       </c>
-      <c r="H74" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3706,10 +4049,10 @@
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E75">
         <v>2019</v>
@@ -3717,14 +4060,18 @@
       <c r="F75" s="1">
         <v>179000</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="1">
+        <f>F75+25000</f>
+        <v>204000</v>
+      </c>
+      <c r="H75">
         <v>69</v>
       </c>
-      <c r="H75" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3732,10 +4079,10 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D76" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E76">
         <v>2018</v>
@@ -3743,14 +4090,18 @@
       <c r="F76" s="1">
         <v>89000</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="1">
+        <f>F76+25000</f>
+        <v>114000</v>
+      </c>
+      <c r="H76">
         <v>4</v>
       </c>
-      <c r="H76" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="I76" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3758,10 +4109,10 @@
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D77" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E77">
         <v>2017</v>
@@ -3769,11 +4120,106 @@
       <c r="F77" s="1">
         <v>79000</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="1">
+        <f>F77+25000</f>
+        <v>104000</v>
+      </c>
+      <c r="H77">
         <v>3</v>
       </c>
-      <c r="H77" s="3" t="s">
-        <v>233</v>
+      <c r="I77" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
+  <cols>
+    <col min="3" max="3" width="25.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="13.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>